<commit_message>
Update ELF and HPEbP with customizations from analysis repo to accomodate BAU hydrogen production
</commit_message>
<xml_diff>
--- a/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
+++ b/InputData/hydgn/HPEbP/Hydgn Production Eff by Pathway.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\hydgn\HPEbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\hydgn\HPEbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5907B1-7D98-49D5-9341-7B22E036D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25820" windowHeight="11970"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="IEA Data" sheetId="3" r:id="rId2"/>
     <sheet name="HPEbP" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -169,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -547,24 +557,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="98.7265625" customWidth="1"/>
+    <col min="2" max="2" width="98.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,120 +582,120 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -693,22 +703,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="F7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="25.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="1" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -728,7 +738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -748,7 +758,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -765,7 +775,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -782,7 +792,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9" t="s">
         <v>28</v>
@@ -800,7 +810,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -820,7 +830,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -837,7 +847,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -854,7 +864,7 @@
         <v>4.7E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="9" t="s">
         <v>30</v>
@@ -872,7 +882,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -892,7 +902,7 @@
         <v>2670</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -909,7 +919,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -926,7 +936,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>30</v>
@@ -944,8 +954,8 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -959,7 +969,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -978,23 +988,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H17:H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>37</v>
       </c>
@@ -1101,7 +1111,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1242,148 +1252,148 @@
         <v>0.77521306818181679</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6">
-        <f>118/(162+2+46)</f>
-        <v>0.56190476190476191</v>
+        <f>118/(162+2)</f>
+        <v>0.71951219512195119</v>
       </c>
       <c r="C3" s="6">
         <f>B3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:O3" si="0">C3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="K3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="L3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="M3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="N3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="O3" s="6">
         <f t="shared" si="0"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="P3" s="13">
         <f>O3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="Q3" s="12">
         <f t="shared" ref="Q3:AI3" si="1">P3</f>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="R3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="S3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="T3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="U3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="V3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="W3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="X3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="Y3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="Z3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AA3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AB3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AC3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AD3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AE3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AF3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AG3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AH3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
+        <v>0.71951219512195119</v>
       </c>
       <c r="AI3" s="12">
         <f t="shared" si="1"/>
-        <v>0.56190476190476191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+        <v>0.71951219512195119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1534,7 @@
         <v>0.57004830917874394</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>0.46274509803921571</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>